<commit_message>
updated script for hcl_cl-
</commit_message>
<xml_diff>
--- a/Cl-_solvated_300K_data.xlsx
+++ b/Cl-_solvated_300K_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/HCl_project_graphs_binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5B5E88-6892-B644-A79C-66612E2EB95E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DD31E4-59A8-864A-B8D5-CEFCE1D30992}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="460" windowWidth="11580" windowHeight="14920" firstSheet="1" activeTab="1" xr2:uid="{66FEA771-CEBD-3F41-A3DD-F4748892B5D8}"/>
+    <workbookView xWindow="1960" yWindow="500" windowWidth="17240" windowHeight="14760" firstSheet="1" activeTab="1" xr2:uid="{66FEA771-CEBD-3F41-A3DD-F4748892B5D8}"/>
   </bookViews>
   <sheets>
     <sheet name="HCl_Cl_longrange_h2om" sheetId="2" r:id="rId1"/>
@@ -989,64 +989,64 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9276A5-8072-C04A-B5F3-2A28797E5081}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>103.98473525</v>
       </c>
@@ -1055,32 +1055,39 @@
         <v>2829.5286308877498</v>
       </c>
       <c r="C9">
+        <f>B9-9.366</f>
+        <v>2820.1626308877499</v>
+      </c>
+      <c r="D9">
         <v>10.150637919999999</v>
       </c>
-      <c r="D9">
-        <f>27.211*C9</f>
+      <c r="E9">
+        <f>27.211*D9</f>
         <v>276.20900844111998</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>7.5546269800000001</v>
       </c>
-      <c r="F9">
-        <f>27.211*E9</f>
+      <c r="G9">
+        <f>27.211*F9</f>
         <v>205.56895475278</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>7.4947800899999999</v>
       </c>
-      <c r="H9">
-        <f>27.211*G9</f>
-        <v>203.94046102898997</v>
-      </c>
       <c r="I9">
-        <f>(F9+H9)/2</f>
-        <v>204.75470789088499</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.4948401699999998</v>
+      </c>
+      <c r="J9">
+        <f>27.211*((H9+I9)/2)</f>
+        <v>203.94127844742997</v>
+      </c>
+      <c r="K9">
+        <f>(G9+J9)/2</f>
+        <v>204.755116600105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>103.98299133</v>
       </c>
@@ -1089,32 +1096,39 @@
         <v>2829.48117708063</v>
       </c>
       <c r="C10">
+        <f t="shared" ref="C10:C58" si="1">B10-9.366</f>
+        <v>2820.11517708063</v>
+      </c>
+      <c r="D10">
         <v>10.14971486</v>
       </c>
-      <c r="D10">
-        <f t="shared" ref="D10:D58" si="1">27.211*C10</f>
+      <c r="E10">
+        <f t="shared" ref="E10:E58" si="2">27.211*D10</f>
         <v>276.18389105545998</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>7.5536330700000001</v>
       </c>
-      <c r="F10">
-        <f t="shared" ref="F10:F58" si="2">27.211*E10</f>
+      <c r="G10">
+        <f t="shared" ref="G10:G58" si="3">27.211*F10</f>
         <v>205.54190946776998</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>7.4937636300000001</v>
       </c>
-      <c r="H10">
-        <f t="shared" ref="H10:H58" si="3">27.211*G10</f>
-        <v>203.91280213592998</v>
-      </c>
       <c r="I10">
-        <f t="shared" ref="I10:I58" si="4">(F10+H10)/2</f>
-        <v>204.72735580184997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.4938792899999997</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10:J58" si="4">27.211*((H10+I10)/2)</f>
+        <v>203.91437574805997</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K58" si="5">(G10+J10)/2</f>
+        <v>204.72814260791498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>104.0059553</v>
       </c>
@@ -1123,32 +1137,39 @@
         <v>2830.1060496682999</v>
       </c>
       <c r="C11">
+        <f t="shared" si="1"/>
+        <v>2820.7400496682999</v>
+      </c>
+      <c r="D11">
         <v>10.17314189</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="1"/>
+      <c r="E11">
+        <f t="shared" si="2"/>
         <v>276.82136396878997</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>7.5770288700000004</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
+      <c r="G11">
+        <f t="shared" si="3"/>
         <v>206.17853258157001</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>7.5171346699999999</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="3"/>
-        <v>204.54875150536998</v>
-      </c>
       <c r="I11">
-        <f t="shared" si="4"/>
-        <v>205.36364204347001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5173053400000001</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>204.551073556055</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="5"/>
+        <v>205.36480306881251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>103.98671074000001</v>
       </c>
@@ -1157,32 +1178,39 @@
         <v>2829.5823859461402</v>
       </c>
       <c r="C12">
+        <f t="shared" si="1"/>
+        <v>2820.2163859461402</v>
+      </c>
+      <c r="D12">
         <v>10.15318381</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="1"/>
+      <c r="E12">
+        <f t="shared" si="2"/>
         <v>276.27828465390996</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>7.5571261600000001</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
+      <c r="G12">
+        <f t="shared" si="3"/>
         <v>205.63695993976</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>7.4972332399999999</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="3"/>
-        <v>204.00721369363998</v>
-      </c>
       <c r="I12">
-        <f t="shared" si="4"/>
-        <v>204.82208681669999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.4973925100000001</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>204.009380641625</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="5"/>
+        <v>204.8231702906925</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>103.99671739999999</v>
       </c>
@@ -1191,32 +1219,39 @@
         <v>2829.8546771713995</v>
       </c>
       <c r="C13">
+        <f t="shared" si="1"/>
+        <v>2820.4886771713996</v>
+      </c>
+      <c r="D13">
         <v>10.16378557</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
+      <c r="E13">
+        <f t="shared" si="2"/>
         <v>276.56676914526997</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>7.5676864500000001</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="2"/>
+      <c r="G13">
+        <f t="shared" si="3"/>
         <v>205.92431599094999</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>7.5078326999999998</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="3"/>
-        <v>204.29563559969998</v>
-      </c>
       <c r="I13">
-        <f t="shared" si="4"/>
-        <v>205.109975795325</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5079215100000001</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>204.296843904155</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="5"/>
+        <v>205.11057994755248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>103.99579859000001</v>
       </c>
@@ -1225,32 +1260,39 @@
         <v>2829.8296754324901</v>
       </c>
       <c r="C14">
+        <f t="shared" si="1"/>
+        <v>2820.4636754324902</v>
+      </c>
+      <c r="D14">
         <v>10.16228499</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="1"/>
+      <c r="E14">
+        <f t="shared" si="2"/>
         <v>276.52593686288998</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>7.5662277199999997</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="2"/>
+      <c r="G14">
+        <f t="shared" si="3"/>
         <v>205.88462248891997</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>7.5063419299999996</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="3"/>
-        <v>204.25507025722999</v>
-      </c>
       <c r="I14">
-        <f t="shared" si="4"/>
-        <v>205.06984637307499</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5064868599999999</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>204.257042102345</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="5"/>
+        <v>205.0708322956325</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>103.99403486</v>
       </c>
@@ -1259,32 +1301,39 @@
         <v>2829.7816825754599</v>
       </c>
       <c r="C15">
+        <f t="shared" si="1"/>
+        <v>2820.4156825754599</v>
+      </c>
+      <c r="D15">
         <v>10.16093223</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="1"/>
+      <c r="E15">
+        <f t="shared" si="2"/>
         <v>276.48912691052999</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>7.5648472900000003</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="2"/>
+      <c r="G15">
+        <f t="shared" si="3"/>
         <v>205.84705960818999</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>7.5049931499999998</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="3"/>
-        <v>204.21836860464998</v>
-      </c>
       <c r="I15">
-        <f t="shared" si="4"/>
-        <v>205.03271410641997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5050802900000004</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>204.21955418791998</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="5"/>
+        <v>205.033306898055</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>103.98802013</v>
       </c>
@@ -1293,32 +1342,39 @@
         <v>2829.6180157574299</v>
       </c>
       <c r="C16">
+        <f t="shared" si="1"/>
+        <v>2820.2520157574299</v>
+      </c>
+      <c r="D16">
         <v>10.153980300000001</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="1"/>
+      <c r="E16">
+        <f t="shared" si="2"/>
         <v>276.2999579433</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>7.5579458600000002</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="2"/>
+      <c r="G16">
+        <f t="shared" si="3"/>
         <v>205.65926479646001</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>7.4980915599999998</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="3"/>
-        <v>204.03056943915999</v>
-      </c>
       <c r="I16">
-        <f t="shared" si="4"/>
-        <v>204.84491711780998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.4981668099999998</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>204.03159325303497</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="5"/>
+        <v>204.84542902474749</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>103.98526914</v>
       </c>
@@ -1327,32 +1383,39 @@
         <v>2829.5431585685396</v>
       </c>
       <c r="C17">
+        <f t="shared" si="1"/>
+        <v>2820.1771585685397</v>
+      </c>
+      <c r="D17">
         <v>10.151753490000001</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="1"/>
+      <c r="E17">
+        <f t="shared" si="2"/>
         <v>276.23936421639002</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>7.5556920400000003</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="2"/>
+      <c r="G17">
+        <f t="shared" si="3"/>
         <v>205.59793610043999</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>7.4957910099999996</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="3"/>
-        <v>203.96796917310996</v>
-      </c>
       <c r="I17">
-        <f t="shared" si="4"/>
-        <v>204.78295263677498</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.4959655100000004</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>203.97034333285998</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="5"/>
+        <v>204.78413971664997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>103.99416803</v>
       </c>
@@ -1361,32 +1424,39 @@
         <v>2829.7853062643298</v>
       </c>
       <c r="C18">
+        <f t="shared" si="1"/>
+        <v>2820.4193062643299</v>
+      </c>
+      <c r="D18">
         <v>10.16123404</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
+      <c r="E18">
+        <f t="shared" si="2"/>
         <v>276.49733946243998</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>7.56513452</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="2"/>
+      <c r="G18">
+        <f t="shared" si="3"/>
         <v>205.85487542371999</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>7.5052550699999996</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="3"/>
-        <v>204.22549570976997</v>
-      </c>
       <c r="I18">
-        <f t="shared" si="4"/>
-        <v>205.04018556674498</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5053949500000003</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="4"/>
+        <v>204.22739884710998</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="5"/>
+        <v>205.041137135415</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>104.00608080000001</v>
       </c>
@@ -1395,32 +1465,39 @@
         <v>2830.1094646488</v>
       </c>
       <c r="C19">
+        <f t="shared" si="1"/>
+        <v>2820.7434646488</v>
+      </c>
+      <c r="D19">
         <v>10.17379749</v>
       </c>
-      <c r="D19">
-        <f t="shared" si="1"/>
+      <c r="E19">
+        <f t="shared" si="2"/>
         <v>276.83920350039</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>7.57764595</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="2"/>
+      <c r="G19">
+        <f t="shared" si="3"/>
         <v>206.19532394544999</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>7.5177875600000004</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="3"/>
-        <v>204.56651729516</v>
-      </c>
       <c r="I19">
-        <f t="shared" si="4"/>
-        <v>205.38092062030501</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5178940499999998</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="4"/>
+        <v>204.56796614485501</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="5"/>
+        <v>205.38164504515248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>103.98972757999999</v>
       </c>
@@ -1429,32 +1506,39 @@
         <v>2829.6644771793794</v>
       </c>
       <c r="C20">
+        <f t="shared" si="1"/>
+        <v>2820.2984771793795</v>
+      </c>
+      <c r="D20">
         <v>10.156872679999999</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
+      <c r="E20">
+        <f t="shared" si="2"/>
         <v>276.37866249547994</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>7.5607593099999999</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="2"/>
+      <c r="G20">
+        <f t="shared" si="3"/>
         <v>205.73582158440999</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>7.50082717</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="3"/>
-        <v>204.10500812286998</v>
-      </c>
       <c r="I20">
-        <f t="shared" si="4"/>
-        <v>204.92041485363998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5010714600000004</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="4"/>
+        <v>204.10833181046499</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="5"/>
+        <v>204.92207669743749</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>104.00212980000001</v>
       </c>
@@ -1463,32 +1547,39 @@
         <v>2830.0019539877999</v>
       </c>
       <c r="C21">
+        <f t="shared" si="1"/>
+        <v>2820.6359539877999</v>
+      </c>
+      <c r="D21">
         <v>10.16844212</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="1"/>
+      <c r="E21">
+        <f t="shared" si="2"/>
         <v>276.69347852732</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>7.5723904299999996</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="2"/>
+      <c r="G21">
+        <f t="shared" si="3"/>
         <v>206.05231599072997</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>7.5125194799999999</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="3"/>
-        <v>204.42316757027999</v>
-      </c>
       <c r="I21">
-        <f t="shared" si="4"/>
-        <v>205.23774178050496</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5126327799999997</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="4"/>
+        <v>204.42470907342997</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="5"/>
+        <v>205.23851253207997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>104.00833797999999</v>
       </c>
@@ -1497,32 +1588,39 @@
         <v>2830.1708847737796</v>
       </c>
       <c r="C22">
+        <f t="shared" si="1"/>
+        <v>2820.8048847737796</v>
+      </c>
+      <c r="D22">
         <v>10.175031000000001</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="1"/>
+      <c r="E22">
+        <f t="shared" si="2"/>
         <v>276.87276854100003</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>7.5789562100000003</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="2"/>
+      <c r="G22">
+        <f t="shared" si="3"/>
         <v>206.23097743030999</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>7.5191793999999996</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="3"/>
-        <v>204.60439065339997</v>
-      </c>
       <c r="I22">
-        <f t="shared" si="4"/>
-        <v>205.41768404185498</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5191099799999996</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="4"/>
+        <v>204.60344615958996</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="5"/>
+        <v>205.41721179494999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>104.00225713</v>
       </c>
@@ -1531,32 +1629,39 @@
         <v>2830.00541876443</v>
       </c>
       <c r="C23">
+        <f t="shared" si="1"/>
+        <v>2820.63941876443</v>
+      </c>
+      <c r="D23">
         <v>10.170237589999999</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="1"/>
+      <c r="E23">
+        <f t="shared" si="2"/>
         <v>276.74233506148994</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>7.5740586499999996</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="2"/>
+      <c r="G23">
+        <f t="shared" si="3"/>
         <v>206.09770992514999</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>7.51423095</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="3"/>
-        <v>204.46973838045</v>
-      </c>
       <c r="I23">
-        <f t="shared" si="4"/>
-        <v>205.2837241528</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5142800899999997</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="4"/>
+        <v>204.47040695471998</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="5"/>
+        <v>205.284058439935</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>104.00408754999999</v>
       </c>
@@ -1565,32 +1670,39 @@
         <v>2830.0552263230497</v>
       </c>
       <c r="C24">
+        <f t="shared" si="1"/>
+        <v>2820.6892263230498</v>
+      </c>
+      <c r="D24">
         <v>10.1698781</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="1"/>
+      <c r="E24">
+        <f t="shared" si="2"/>
         <v>276.73255297909998</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>7.57387751</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="2"/>
+      <c r="G24">
+        <f t="shared" si="3"/>
         <v>206.09278092461</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>7.51400413</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="3"/>
-        <v>204.46356638142998</v>
-      </c>
       <c r="I24">
-        <f t="shared" si="4"/>
-        <v>205.27817365301999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5141156499999999</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="4"/>
+        <v>204.46508366679001</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="5"/>
+        <v>205.2789322957</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>104.00474136</v>
       </c>
@@ -1599,32 +1711,39 @@
         <v>2830.07301714696</v>
       </c>
       <c r="C25">
+        <f t="shared" si="1"/>
+        <v>2820.70701714696</v>
+      </c>
+      <c r="D25">
         <v>10.172495850000001</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="1"/>
+      <c r="E25">
+        <f t="shared" si="2"/>
         <v>276.80378457435</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>7.5763329099999996</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="2"/>
+      <c r="G25">
+        <f t="shared" si="3"/>
         <v>206.15959481400998</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>7.5164378200000002</v>
       </c>
-      <c r="H25">
-        <f t="shared" si="3"/>
-        <v>204.52978952001999</v>
-      </c>
       <c r="I25">
-        <f t="shared" si="4"/>
-        <v>205.34469216701498</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5166175400000004</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="4"/>
+        <v>204.53223470047999</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="5"/>
+        <v>205.345914757245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>103.97023485</v>
       </c>
@@ -1633,32 +1752,39 @@
         <v>2829.1340605033497</v>
       </c>
       <c r="C26">
+        <f t="shared" si="1"/>
+        <v>2819.7680605033497</v>
+      </c>
+      <c r="D26">
         <v>10.13637102</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="1"/>
+      <c r="E26">
+        <f t="shared" si="2"/>
         <v>275.82079182522</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>7.5403216400000002</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="2"/>
+      <c r="G26">
+        <f t="shared" si="3"/>
         <v>205.17969214604</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>7.4804511800000002</v>
       </c>
-      <c r="H26">
-        <f t="shared" si="3"/>
-        <v>203.55055705897999</v>
-      </c>
       <c r="I26">
-        <f t="shared" si="4"/>
-        <v>204.36512460250998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.48056053</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="4"/>
+        <v>203.552044820405</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="5"/>
+        <v>204.3658684832225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>104.01752596999999</v>
       </c>
@@ -1667,32 +1793,39 @@
         <v>2830.4208991696696</v>
       </c>
       <c r="C27">
+        <f t="shared" si="1"/>
+        <v>2821.0548991696696</v>
+      </c>
+      <c r="D27">
         <v>10.18500822</v>
       </c>
-      <c r="D27">
-        <f t="shared" si="1"/>
+      <c r="E27">
+        <f t="shared" si="2"/>
         <v>277.14425867441997</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>7.5888774100000003</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="2"/>
+      <c r="G27">
+        <f t="shared" si="3"/>
         <v>206.50094320350999</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>7.5289709</v>
       </c>
-      <c r="H27">
-        <f t="shared" si="3"/>
-        <v>204.87082715989999</v>
-      </c>
       <c r="I27">
-        <f t="shared" si="4"/>
-        <v>205.68588518170498</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5291697099999997</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="4"/>
+        <v>204.87353206935498</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="5"/>
+        <v>205.68723763643249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>104.00544352</v>
       </c>
@@ -1701,32 +1834,39 @@
         <v>2830.09212362272</v>
       </c>
       <c r="C28">
+        <f t="shared" si="1"/>
+        <v>2820.72612362272</v>
+      </c>
+      <c r="D28">
         <v>10.17212988</v>
       </c>
-      <c r="D28">
-        <f t="shared" si="1"/>
+      <c r="E28">
+        <f t="shared" si="2"/>
         <v>276.79382616467996</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>7.5760581599999997</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="2"/>
+      <c r="G28">
+        <f t="shared" si="3"/>
         <v>206.15211859175997</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>7.5162133200000003</v>
       </c>
-      <c r="H28">
-        <f t="shared" si="3"/>
-        <v>204.52368065051999</v>
-      </c>
       <c r="I28">
-        <f t="shared" si="4"/>
-        <v>205.33789962113997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5162795300000003</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="4"/>
+        <v>204.524581470675</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="5"/>
+        <v>205.33835003121749</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>103.98661076</v>
       </c>
@@ -1735,32 +1875,39 @@
         <v>2829.5796653903599</v>
       </c>
       <c r="C29">
+        <f t="shared" si="1"/>
+        <v>2820.2136653903599</v>
+      </c>
+      <c r="D29">
         <v>10.15305034</v>
       </c>
-      <c r="D29">
-        <f t="shared" si="1"/>
+      <c r="E29">
+        <f t="shared" si="2"/>
         <v>276.27465280173999</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>7.55698633</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="2"/>
+      <c r="G29">
+        <f t="shared" si="3"/>
         <v>205.63315502562997</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>7.4971105800000002</v>
       </c>
-      <c r="H29">
-        <f t="shared" si="3"/>
-        <v>204.00387599237999</v>
-      </c>
       <c r="I29">
-        <f t="shared" si="4"/>
-        <v>204.81851550900498</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.4972345799999998</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="4"/>
+        <v>204.00556307437998</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="5"/>
+        <v>204.81935905000498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>103.99883495</v>
       </c>
@@ -1769,32 +1916,39 @@
         <v>2829.91229782445</v>
       </c>
       <c r="C30">
+        <f t="shared" si="1"/>
+        <v>2820.54629782445</v>
+      </c>
+      <c r="D30">
         <v>10.16656302</v>
       </c>
-      <c r="D30">
-        <f t="shared" si="1"/>
+      <c r="E30">
+        <f t="shared" si="2"/>
         <v>276.64234633721998</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>7.57041509</v>
       </c>
-      <c r="F30">
-        <f t="shared" si="2"/>
+      <c r="G30">
+        <f t="shared" si="3"/>
         <v>205.99856501399</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>7.5106895700000003</v>
       </c>
-      <c r="H30">
-        <f t="shared" si="3"/>
-        <v>204.37337388927</v>
-      </c>
       <c r="I30">
-        <f t="shared" si="4"/>
-        <v>205.18596945163</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5105301400000002</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="4"/>
+        <v>204.37120476440501</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="5"/>
+        <v>205.18488488919752</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>103.99220627</v>
       </c>
@@ -1803,32 +1957,39 @@
         <v>2829.7319248129697</v>
       </c>
       <c r="C31">
+        <f t="shared" si="1"/>
+        <v>2820.3659248129698</v>
+      </c>
+      <c r="D31">
         <v>10.158899659999999</v>
       </c>
-      <c r="D31">
-        <f t="shared" si="1"/>
+      <c r="E31">
+        <f t="shared" si="2"/>
         <v>276.43381864825994</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>7.5628239300000004</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="2"/>
+      <c r="G31">
+        <f t="shared" si="3"/>
         <v>205.79200195922999</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>7.5029631700000001</v>
       </c>
-      <c r="H31">
-        <f t="shared" si="3"/>
-        <v>204.16313081887</v>
-      </c>
       <c r="I31">
-        <f t="shared" si="4"/>
-        <v>204.97756638905</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5030607500000004</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="4"/>
+        <v>204.16445844355999</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="5"/>
+        <v>204.97823020139498</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>104.01414741000001</v>
       </c>
@@ -1837,32 +1998,39 @@
         <v>2830.3289651735099</v>
       </c>
       <c r="C32">
+        <f t="shared" si="1"/>
+        <v>2820.9629651735099</v>
+      </c>
+      <c r="D32">
         <v>10.180524139999999</v>
       </c>
-      <c r="D32">
-        <f t="shared" si="1"/>
+      <c r="E32">
+        <f t="shared" si="2"/>
         <v>277.02224237353994</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>7.5844770300000004</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="2"/>
+      <c r="G32">
+        <f t="shared" si="3"/>
         <v>206.38120446332999</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>7.5246307000000003</v>
       </c>
-      <c r="H32">
-        <f t="shared" si="3"/>
-        <v>204.75272597770001</v>
-      </c>
       <c r="I32">
-        <f t="shared" si="4"/>
-        <v>205.56696522051499</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5246960100000004</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="4"/>
+        <v>204.75361455290499</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="5"/>
+        <v>205.56740950811749</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>103.99460759999999</v>
       </c>
@@ -1871,32 +2039,39 @@
         <v>2829.7972674035996</v>
       </c>
       <c r="C33">
+        <f t="shared" si="1"/>
+        <v>2820.4312674035996</v>
+      </c>
+      <c r="D33">
         <v>10.16117453</v>
       </c>
-      <c r="D33">
-        <f t="shared" si="1"/>
+      <c r="E33">
+        <f t="shared" si="2"/>
         <v>276.49572013582997</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>7.5651131300000003</v>
       </c>
-      <c r="F33">
-        <f t="shared" si="2"/>
+      <c r="G33">
+        <f t="shared" si="3"/>
         <v>205.85429338042999</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>7.5052559299999997</v>
       </c>
-      <c r="H33">
-        <f t="shared" si="3"/>
-        <v>204.22551911122997</v>
-      </c>
       <c r="I33">
-        <f t="shared" si="4"/>
-        <v>205.03990624582997</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5053452900000002</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="4"/>
+        <v>204.22673489870999</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="5"/>
+        <v>205.04051413957001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>103.99087486000001</v>
       </c>
@@ -1905,32 +2080,39 @@
         <v>2829.6956958154601</v>
       </c>
       <c r="C34">
+        <f t="shared" si="1"/>
+        <v>2820.3296958154601</v>
+      </c>
+      <c r="D34">
         <v>10.158088899999999</v>
       </c>
-      <c r="D34">
-        <f t="shared" si="1"/>
+      <c r="E34">
+        <f t="shared" si="2"/>
         <v>276.41175705789999</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>7.5619679299999998</v>
       </c>
-      <c r="F34">
-        <f t="shared" si="2"/>
+      <c r="G34">
+        <f t="shared" si="3"/>
         <v>205.76870934322997</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>7.5020710299999998</v>
       </c>
-      <c r="H34">
-        <f t="shared" si="3"/>
-        <v>204.13885479732997</v>
-      </c>
       <c r="I34">
-        <f t="shared" si="4"/>
-        <v>204.95378207027997</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5022475699999998</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="4"/>
+        <v>204.14125671229999</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="5"/>
+        <v>204.95498302776497</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>104.01962825</v>
       </c>
@@ -1939,32 +2121,39 @@
         <v>2830.4781043107496</v>
       </c>
       <c r="C35">
+        <f t="shared" si="1"/>
+        <v>2821.1121043107496</v>
+      </c>
+      <c r="D35">
         <v>10.185878089999999</v>
       </c>
-      <c r="D35">
-        <f t="shared" si="1"/>
+      <c r="E35">
+        <f t="shared" si="2"/>
         <v>277.16792870698998</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>7.5898258399999996</v>
       </c>
-      <c r="F35">
-        <f t="shared" si="2"/>
+      <c r="G35">
+        <f t="shared" si="3"/>
         <v>206.52675093223999</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>7.5299773600000002</v>
       </c>
-      <c r="H35">
-        <f t="shared" si="3"/>
-        <v>204.89821394295998</v>
-      </c>
       <c r="I35">
-        <f t="shared" si="4"/>
-        <v>205.71248243759999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5300451800000001</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="4"/>
+        <v>204.89913666797</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="5"/>
+        <v>205.71294380010499</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>104.0033183</v>
       </c>
@@ -1973,32 +2162,39 @@
         <v>2830.0342942613001</v>
       </c>
       <c r="C36">
+        <f t="shared" si="1"/>
+        <v>2820.6682942613002</v>
+      </c>
+      <c r="D36">
         <v>10.17050341</v>
       </c>
-      <c r="D36">
-        <f t="shared" si="1"/>
+      <c r="E36">
+        <f t="shared" si="2"/>
         <v>276.74956828950997</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>7.5743872000000003</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="2"/>
+      <c r="G36">
+        <f t="shared" si="3"/>
         <v>206.10665009920001</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>7.5145456199999998</v>
       </c>
-      <c r="H36">
-        <f t="shared" si="3"/>
-        <v>204.47830086581999</v>
-      </c>
       <c r="I36">
-        <f t="shared" si="4"/>
-        <v>205.29247548250999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5146118199999998</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="4"/>
+        <v>204.47920154991996</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="5"/>
+        <v>205.29292582455997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>104.00963387</v>
       </c>
@@ -2007,32 +2203,39 @@
         <v>2830.2061472365699</v>
       </c>
       <c r="C37">
+        <f t="shared" si="1"/>
+        <v>2820.8401472365699</v>
+      </c>
+      <c r="D37">
         <v>10.176098870000001</v>
       </c>
-      <c r="D37">
-        <f t="shared" si="1"/>
+      <c r="E37">
+        <f t="shared" si="2"/>
         <v>276.90182635156998</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>7.5800369200000004</v>
       </c>
-      <c r="F37">
-        <f t="shared" si="2"/>
+      <c r="G37">
+        <f t="shared" si="3"/>
         <v>206.26038463012</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>7.5201760699999998</v>
       </c>
-      <c r="H37">
-        <f t="shared" si="3"/>
-        <v>204.63151104076999</v>
-      </c>
       <c r="I37">
-        <f t="shared" si="4"/>
-        <v>205.445947835445</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5202705700000001</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="4"/>
+        <v>204.63279676051997</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="5"/>
+        <v>205.44659069531997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>104.00124266</v>
       </c>
@@ -2041,32 +2244,39 @@
         <v>2829.9778140212597</v>
       </c>
       <c r="C38">
+        <f t="shared" si="1"/>
+        <v>2820.6118140212598</v>
+      </c>
+      <c r="D38">
         <v>10.168234590000001</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="1"/>
+      <c r="E38">
+        <f t="shared" si="2"/>
         <v>276.68783142849003</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>7.5721326299999996</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="2"/>
+      <c r="G38">
+        <f t="shared" si="3"/>
         <v>206.04530099492999</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>7.5122497299999997</v>
       </c>
-      <c r="H38">
-        <f t="shared" si="3"/>
-        <v>204.41582740302999</v>
-      </c>
       <c r="I38">
-        <f t="shared" si="4"/>
-        <v>205.23056419898001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5123955899999997</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="4"/>
+        <v>204.41781190126</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="5"/>
+        <v>205.23155644809498</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>104.02006839000001</v>
       </c>
@@ -2075,32 +2285,39 @@
         <v>2830.49008096029</v>
       </c>
       <c r="C39">
+        <f t="shared" si="1"/>
+        <v>2821.12408096029</v>
+      </c>
+      <c r="D39">
         <v>10.18722419</v>
       </c>
-      <c r="D39">
-        <f t="shared" si="1"/>
+      <c r="E39">
+        <f t="shared" si="2"/>
         <v>277.20455743408996</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>7.5911154600000001</v>
       </c>
-      <c r="F39">
-        <f t="shared" si="2"/>
+      <c r="G39">
+        <f t="shared" si="3"/>
         <v>206.56184278205998</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>7.53122208</v>
       </c>
-      <c r="H39">
-        <f t="shared" si="3"/>
-        <v>204.93208401887998</v>
-      </c>
       <c r="I39">
-        <f t="shared" si="4"/>
-        <v>205.74696340046998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5313908899999999</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="4"/>
+        <v>204.93438076333499</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="5"/>
+        <v>205.74811177269748</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>104.00239911</v>
       </c>
@@ -2109,32 +2326,39 @@
         <v>2830.00928218221</v>
       </c>
       <c r="C40">
+        <f t="shared" si="1"/>
+        <v>2820.64328218221</v>
+      </c>
+      <c r="D40">
         <v>10.170092009999999</v>
       </c>
-      <c r="D40">
-        <f t="shared" si="1"/>
+      <c r="E40">
+        <f t="shared" si="2"/>
         <v>276.73837368410994</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>7.5739413200000003</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="2"/>
+      <c r="G40">
+        <f t="shared" si="3"/>
         <v>206.09451725852</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>7.5140863400000004</v>
       </c>
-      <c r="H40">
-        <f t="shared" si="3"/>
-        <v>204.46580339773999</v>
-      </c>
       <c r="I40">
-        <f t="shared" si="4"/>
-        <v>205.28016032812999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5141856499999999</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="4"/>
+        <v>204.46715455994499</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="5"/>
+        <v>205.28083590923251</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>104.00745857</v>
       </c>
@@ -2143,32 +2367,39 @@
         <v>2830.1469551482696</v>
       </c>
       <c r="C41">
+        <f t="shared" si="1"/>
+        <v>2820.7809551482696</v>
+      </c>
+      <c r="D41">
         <v>10.17445186</v>
       </c>
-      <c r="D41">
-        <f t="shared" si="1"/>
+      <c r="E41">
+        <f t="shared" si="2"/>
         <v>276.85700956245995</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>7.57835299</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="2"/>
+      <c r="G41">
+        <f t="shared" si="3"/>
         <v>206.21456321088999</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>7.5184637499999996</v>
       </c>
-      <c r="H41">
-        <f t="shared" si="3"/>
-        <v>204.58491710124997</v>
-      </c>
       <c r="I41">
-        <f t="shared" si="4"/>
-        <v>205.39974015606998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5186222300000001</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="4"/>
+        <v>204.58707330088998</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="5"/>
+        <v>205.40081825588999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>104.00634994000001</v>
       </c>
@@ -2177,32 +2408,39 @@
         <v>2830.1167882173399</v>
       </c>
       <c r="C42">
+        <f t="shared" si="1"/>
+        <v>2820.75078821734</v>
+      </c>
+      <c r="D42">
         <v>10.173771090000001</v>
       </c>
-      <c r="D42">
-        <f t="shared" si="1"/>
+      <c r="E42">
+        <f t="shared" si="2"/>
         <v>276.83848512998998</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>7.5776437799999998</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="2"/>
+      <c r="G42">
+        <f t="shared" si="3"/>
         <v>206.19526489757999</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>7.5179042899999997</v>
       </c>
-      <c r="H42">
-        <f t="shared" si="3"/>
-        <v>204.56969363518999</v>
-      </c>
       <c r="I42">
-        <f t="shared" si="4"/>
-        <v>205.38247926638499</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5177695599999996</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="4"/>
+        <v>204.56786056617497</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="5"/>
+        <v>205.38156273187747</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>103.99814326000001</v>
       </c>
@@ -2211,32 +2449,39 @@
         <v>2829.8934762478602</v>
       </c>
       <c r="C43">
+        <f t="shared" si="1"/>
+        <v>2820.5274762478602</v>
+      </c>
+      <c r="D43">
         <v>10.16568724</v>
       </c>
-      <c r="D43">
-        <f t="shared" si="1"/>
+      <c r="E43">
+        <f t="shared" si="2"/>
         <v>276.61851548764002</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>7.5695475600000002</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="2"/>
+      <c r="G43">
+        <f t="shared" si="3"/>
         <v>205.97495865515998</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>7.50968956</v>
       </c>
-      <c r="H43">
-        <f t="shared" si="3"/>
-        <v>204.34616261715999</v>
-      </c>
       <c r="I43">
-        <f t="shared" si="4"/>
-        <v>205.16056063615997</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5097935400000004</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="4"/>
+        <v>204.34757731705</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="5"/>
+        <v>205.16126798610497</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>103.99047633000001</v>
       </c>
@@ -2245,32 +2490,39 @@
         <v>2829.68485141563</v>
       </c>
       <c r="C44">
+        <f t="shared" si="1"/>
+        <v>2820.31885141563</v>
+      </c>
+      <c r="D44">
         <v>10.15780251</v>
       </c>
-      <c r="D44">
-        <f t="shared" si="1"/>
+      <c r="E44">
+        <f t="shared" si="2"/>
         <v>276.40396409960999</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>7.5616841399999997</v>
       </c>
-      <c r="F44">
-        <f t="shared" si="2"/>
+      <c r="G44">
+        <f t="shared" si="3"/>
         <v>205.76098713353997</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>7.5017822399999998</v>
       </c>
-      <c r="H44">
-        <f t="shared" si="3"/>
-        <v>204.13099653263998</v>
-      </c>
       <c r="I44">
-        <f t="shared" si="4"/>
-        <v>204.94599183308998</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5019698899999998</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="4"/>
+        <v>204.13354960471497</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="5"/>
+        <v>204.94726836912747</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>104.01855944</v>
       </c>
@@ -2279,32 +2531,39 @@
         <v>2830.4490209218397</v>
       </c>
       <c r="C45">
+        <f t="shared" si="1"/>
+        <v>2821.0830209218398</v>
+      </c>
+      <c r="D45">
         <v>10.18510824</v>
       </c>
-      <c r="D45">
-        <f t="shared" si="1"/>
+      <c r="E45">
+        <f t="shared" si="2"/>
         <v>277.14698031863998</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>7.5890495700000002</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="2"/>
+      <c r="G45">
+        <f t="shared" si="3"/>
         <v>206.50562784926998</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>7.5291680699999999</v>
       </c>
-      <c r="H45">
-        <f t="shared" si="3"/>
-        <v>204.87619235276998</v>
-      </c>
       <c r="I45">
-        <f t="shared" si="4"/>
-        <v>205.69091010101999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5293060199999999</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="4"/>
+        <v>204.878069231495</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="5"/>
+        <v>205.69184854038249</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>104.00102812999999</v>
       </c>
@@ -2313,32 +2572,39 @@
         <v>2829.9719764454298</v>
       </c>
       <c r="C46">
+        <f t="shared" si="1"/>
+        <v>2820.6059764454299</v>
+      </c>
+      <c r="D46">
         <v>10.168387620000001</v>
       </c>
-      <c r="D46">
-        <f t="shared" si="1"/>
+      <c r="E46">
+        <f t="shared" si="2"/>
         <v>276.69199552781998</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>7.5722522799999998</v>
       </c>
-      <c r="F46">
-        <f t="shared" si="2"/>
+      <c r="G46">
+        <f t="shared" si="3"/>
         <v>206.04855679107999</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>7.5123582899999999</v>
       </c>
-      <c r="H46">
-        <f t="shared" si="3"/>
-        <v>204.41878142918998</v>
-      </c>
       <c r="I46">
-        <f t="shared" si="4"/>
-        <v>205.233669110135</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5125305899999999</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="4"/>
+        <v>204.42112565683996</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="5"/>
+        <v>205.23484122395996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>103.98558782000001</v>
       </c>
@@ -2347,32 +2613,39 @@
         <v>2829.5518301700199</v>
       </c>
       <c r="C47">
+        <f t="shared" si="1"/>
+        <v>2820.1858301700199</v>
+      </c>
+      <c r="D47">
         <v>10.1523419</v>
       </c>
-      <c r="D47">
-        <f t="shared" si="1"/>
+      <c r="E47">
+        <f t="shared" si="2"/>
         <v>276.25537544089997</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>7.5562669500000004</v>
       </c>
-      <c r="F47">
-        <f t="shared" si="2"/>
+      <c r="G47">
+        <f t="shared" si="3"/>
         <v>205.61357997645001</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>7.4963787200000001</v>
       </c>
-      <c r="H47">
-        <f t="shared" si="3"/>
-        <v>203.98396134991998</v>
-      </c>
       <c r="I47">
-        <f t="shared" si="4"/>
-        <v>204.798770663185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.4965314699999999</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="4"/>
+        <v>203.98603959004498</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="5"/>
+        <v>204.7998097832475</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>103.97663944</v>
       </c>
@@ -2381,32 +2654,39 @@
         <v>2829.3083358018398</v>
       </c>
       <c r="C48">
+        <f t="shared" si="1"/>
+        <v>2819.9423358018398</v>
+      </c>
+      <c r="D48">
         <v>10.142994209999999</v>
       </c>
-      <c r="D48">
-        <f t="shared" si="1"/>
+      <c r="E48">
+        <f t="shared" si="2"/>
         <v>276.00101544830994</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>7.5469489300000001</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="2"/>
+      <c r="G48">
+        <f t="shared" si="3"/>
         <v>205.36002733422998</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>7.4870922499999999</v>
       </c>
-      <c r="H48">
-        <f t="shared" si="3"/>
-        <v>203.73126721474998</v>
-      </c>
       <c r="I48">
-        <f t="shared" si="4"/>
-        <v>204.54564727448997</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.4871774899999997</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="4"/>
+        <v>203.73242694756999</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="5"/>
+        <v>204.54622714089999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>103.99689286</v>
       </c>
@@ -2415,32 +2695,39 @@
         <v>2829.8594516134599</v>
       </c>
       <c r="C49">
+        <f t="shared" si="1"/>
+        <v>2820.4934516134599</v>
+      </c>
+      <c r="D49">
         <v>10.16325973</v>
       </c>
-      <c r="D49">
-        <f t="shared" si="1"/>
+      <c r="E49">
+        <f t="shared" si="2"/>
         <v>276.55246051302998</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>7.5672184199999997</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="2"/>
+      <c r="G49">
+        <f t="shared" si="3"/>
         <v>205.91158042661999</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>7.50730232</v>
       </c>
-      <c r="H49">
-        <f t="shared" si="3"/>
-        <v>204.28120342951999</v>
-      </c>
       <c r="I49">
-        <f t="shared" si="4"/>
-        <v>205.09639192806998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5075053900000004</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="4"/>
+        <v>204.28396629840498</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="5"/>
+        <v>205.0977733625125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>103.97791442</v>
       </c>
@@ -2449,32 +2736,39 @@
         <v>2829.3430292826201</v>
       </c>
       <c r="C50">
+        <f t="shared" si="1"/>
+        <v>2819.9770292826202</v>
+      </c>
+      <c r="D50">
         <v>10.144490230000001</v>
       </c>
-      <c r="D50">
-        <f t="shared" si="1"/>
+      <c r="E50">
+        <f t="shared" si="2"/>
         <v>276.04172364853002</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>7.54842368</v>
       </c>
-      <c r="F50">
-        <f t="shared" si="2"/>
+      <c r="G50">
+        <f t="shared" si="3"/>
         <v>205.40015675647999</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>7.4886473999999996</v>
       </c>
-      <c r="H50">
-        <f t="shared" si="3"/>
-        <v>203.77358440139997</v>
-      </c>
       <c r="I50">
-        <f t="shared" si="4"/>
-        <v>204.58687057893997</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.4885745300000002</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="4"/>
+        <v>203.77259296861499</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="5"/>
+        <v>204.58637486254747</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>104.00561768999999</v>
       </c>
@@ -2483,32 +2777,39 @@
         <v>2830.0968629625895</v>
       </c>
       <c r="C51">
+        <f t="shared" si="1"/>
+        <v>2820.7308629625895</v>
+      </c>
+      <c r="D51">
         <v>10.172658520000001</v>
       </c>
-      <c r="D51">
-        <f t="shared" si="1"/>
+      <c r="E51">
+        <f t="shared" si="2"/>
         <v>276.80821098771997</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>7.5765606500000002</v>
       </c>
-      <c r="F51">
-        <f t="shared" si="2"/>
+      <c r="G51">
+        <f t="shared" si="3"/>
         <v>206.16579184714999</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>7.5166822800000004</v>
       </c>
-      <c r="H51">
-        <f t="shared" si="3"/>
-        <v>204.53644152108001</v>
-      </c>
       <c r="I51">
-        <f t="shared" si="4"/>
-        <v>205.351116684115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5168202400000004</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="4"/>
+        <v>204.53831853585999</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="5"/>
+        <v>205.35205519150497</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>104.01195380999999</v>
       </c>
@@ -2517,32 +2818,39 @@
         <v>2830.2692751239097</v>
       </c>
       <c r="C52">
+        <f t="shared" si="1"/>
+        <v>2820.9032751239097</v>
+      </c>
+      <c r="D52">
         <v>10.178386120000001</v>
       </c>
-      <c r="D52">
-        <f t="shared" si="1"/>
+      <c r="E52">
+        <f t="shared" si="2"/>
         <v>276.96406471132002</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>7.5823318300000002</v>
       </c>
-      <c r="F52">
-        <f t="shared" si="2"/>
+      <c r="G52">
+        <f t="shared" si="3"/>
         <v>206.32283142612999</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>7.5224683600000004</v>
       </c>
-      <c r="H52">
-        <f t="shared" si="3"/>
-        <v>204.69388654395999</v>
-      </c>
       <c r="I52">
-        <f t="shared" si="4"/>
-        <v>205.50835898504499</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5225687099999998</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="4"/>
+        <v>204.69525185588498</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="5"/>
+        <v>205.50904164100749</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>104.01132001000001</v>
       </c>
@@ -2551,32 +2859,39 @@
         <v>2830.2520287921102</v>
       </c>
       <c r="C53">
+        <f t="shared" si="1"/>
+        <v>2820.8860287921102</v>
+      </c>
+      <c r="D53">
         <v>10.178216089999999</v>
       </c>
-      <c r="D53">
-        <f t="shared" si="1"/>
+      <c r="E53">
+        <f t="shared" si="2"/>
         <v>276.95943802498999</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>7.5821249499999999</v>
       </c>
-      <c r="F53">
-        <f t="shared" si="2"/>
+      <c r="G53">
+        <f t="shared" si="3"/>
         <v>206.31720201444998</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>7.5222647199999999</v>
       </c>
-      <c r="H53">
-        <f t="shared" si="3"/>
-        <v>204.68834529591999</v>
-      </c>
       <c r="I53">
-        <f t="shared" si="4"/>
-        <v>205.50277365518497</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5223646999999998</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="4"/>
+        <v>204.68970557380999</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="5"/>
+        <v>205.50345379413</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>104.01455815</v>
       </c>
@@ -2585,32 +2900,39 @@
         <v>2830.3401418196499</v>
       </c>
       <c r="C54">
+        <f t="shared" si="1"/>
+        <v>2820.97414181965</v>
+      </c>
+      <c r="D54">
         <v>10.182062350000001</v>
       </c>
-      <c r="D54">
-        <f t="shared" si="1"/>
+      <c r="E54">
+        <f t="shared" si="2"/>
         <v>277.06409860585001</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>7.5859250899999999</v>
       </c>
-      <c r="F54">
-        <f t="shared" si="2"/>
+      <c r="G54">
+        <f t="shared" si="3"/>
         <v>206.42060762398998</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>7.5260718500000001</v>
       </c>
-      <c r="H54">
-        <f t="shared" si="3"/>
-        <v>204.79194111035</v>
-      </c>
       <c r="I54">
-        <f t="shared" si="4"/>
-        <v>205.60627436716999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5261656099999996</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="4"/>
+        <v>204.79321676203</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="5"/>
+        <v>205.60691219300998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>104.02132354</v>
       </c>
@@ -2619,32 +2941,39 @@
         <v>2830.5242348469396</v>
       </c>
       <c r="C55">
+        <f t="shared" si="1"/>
+        <v>2821.1582348469396</v>
+      </c>
+      <c r="D55">
         <v>10.18895118</v>
       </c>
-      <c r="D55">
-        <f t="shared" si="1"/>
+      <c r="E55">
+        <f t="shared" si="2"/>
         <v>277.25155055898</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>7.5927998399999996</v>
       </c>
-      <c r="F55">
-        <f t="shared" si="2"/>
+      <c r="G55">
+        <f t="shared" si="3"/>
         <v>206.60767644623999</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>7.5329499599999998</v>
       </c>
-      <c r="H55">
-        <f t="shared" si="3"/>
-        <v>204.97910136156</v>
-      </c>
       <c r="I55">
-        <f t="shared" si="4"/>
-        <v>205.7933889039</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.5330385900000003</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="4"/>
+        <v>204.980307217025</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="5"/>
+        <v>205.7939918316325</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>104.00636572000001</v>
       </c>
@@ -2653,32 +2982,39 @@
         <v>2830.1172176069199</v>
       </c>
       <c r="C56">
+        <f t="shared" si="1"/>
+        <v>2820.7512176069199</v>
+      </c>
+      <c r="D56">
         <v>10.17298166</v>
       </c>
-      <c r="D56">
-        <f t="shared" si="1"/>
+      <c r="E56">
+        <f t="shared" si="2"/>
         <v>276.81700395025996</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>7.5769138399999996</v>
       </c>
-      <c r="F56">
-        <f t="shared" si="2"/>
+      <c r="G56">
+        <f t="shared" si="3"/>
         <v>206.17540250023998</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>7.5170501099999996</v>
       </c>
-      <c r="H56">
-        <f t="shared" si="3"/>
-        <v>204.54645054320997</v>
-      </c>
       <c r="I56">
-        <f t="shared" si="4"/>
-        <v>205.36092652172499</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.51715292</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="4"/>
+        <v>204.54784932466501</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="5"/>
+        <v>205.3616259124525</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>103.98306853</v>
       </c>
@@ -2687,32 +3023,39 @@
         <v>2829.4832777698298</v>
       </c>
       <c r="C57">
+        <f t="shared" si="1"/>
+        <v>2820.1172777698298</v>
+      </c>
+      <c r="D57">
         <v>10.15019927</v>
       </c>
-      <c r="D57">
-        <f t="shared" si="1"/>
+      <c r="E57">
+        <f t="shared" si="2"/>
         <v>276.19707233597001</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>7.5540906799999998</v>
       </c>
-      <c r="F57">
-        <f t="shared" si="2"/>
+      <c r="G57">
+        <f t="shared" si="3"/>
         <v>205.55436149347997</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>7.4943012199999997</v>
       </c>
-      <c r="H57">
-        <f t="shared" si="3"/>
-        <v>203.92743049741998</v>
-      </c>
       <c r="I57">
-        <f t="shared" si="4"/>
-        <v>204.74089599544999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7.4942618599999999</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="4"/>
+        <v>203.92689498493996</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="5"/>
+        <v>204.74062823920997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>103.99570208999999</v>
       </c>
@@ -2721,29 +3064,36 @@
         <v>2829.8270495709899</v>
       </c>
       <c r="C58">
+        <f t="shared" si="1"/>
+        <v>2820.4610495709899</v>
+      </c>
+      <c r="D58">
         <v>10.16211322</v>
       </c>
-      <c r="D58">
-        <f t="shared" si="1"/>
+      <c r="E58">
+        <f t="shared" si="2"/>
         <v>276.52126282941998</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>7.5660607400000002</v>
       </c>
-      <c r="F58">
-        <f t="shared" si="2"/>
+      <c r="G58">
+        <f t="shared" si="3"/>
         <v>205.88007879614</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>7.5061937700000003</v>
       </c>
-      <c r="H58">
-        <f t="shared" si="3"/>
-        <v>204.25103867547</v>
-      </c>
       <c r="I58">
-        <f t="shared" si="4"/>
-        <v>205.06555873580498</v>
+        <v>7.5063002900000004</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="4"/>
+        <v>204.25248793333</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="5"/>
+        <v>205.066283364735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>